<commit_message>
feat: update complete project with latest Streamlit version
</commit_message>
<xml_diff>
--- a/data/ingredients_final.xlsx
+++ b/data/ingredients_final.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yamine\Documents\fiche-technique-streamlit\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1102C09A-B26B-427A-B7A4-5B2F1FA0C63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$121</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="52">
   <si>
     <t>plat</t>
   </si>
@@ -73,6 +82,12 @@
     <t>Truffe M</t>
   </si>
   <si>
+    <t>panini pizz base crème</t>
+  </si>
+  <si>
+    <t>panini pizz base tomate</t>
+  </si>
+  <si>
     <t>Crème</t>
   </si>
   <si>
@@ -119,6 +134,48 @@
   </si>
   <si>
     <t>Parmesan</t>
+  </si>
+  <si>
+    <t>sauce tomate</t>
+  </si>
+  <si>
+    <t>janbon blanc</t>
+  </si>
+  <si>
+    <t>chorizo</t>
+  </si>
+  <si>
+    <t>Bœuf</t>
+  </si>
+  <si>
+    <t>Merguez</t>
+  </si>
+  <si>
+    <t>Poivron</t>
+  </si>
+  <si>
+    <t>Olive</t>
+  </si>
+  <si>
+    <t>Piment</t>
+  </si>
+  <si>
+    <t>Lardon</t>
+  </si>
+  <si>
+    <t>Artichaut</t>
+  </si>
+  <si>
+    <t>Capre</t>
+  </si>
+  <si>
+    <t>T.C</t>
+  </si>
+  <si>
+    <t>Thon</t>
+  </si>
+  <si>
+    <t>Auber</t>
   </si>
   <si>
     <t>g</t>
@@ -127,8 +184,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,13 +248,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +300,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -269,6 +334,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -303,9 +369,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,14 +545,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,1197 +575,2048 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E2">
         <v>3.75</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E3">
         <v>5.85</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>10.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E7">
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>5.85</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>10.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E12">
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>5.85</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E14">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>1.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E16">
         <v>3.75</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E17">
         <v>5.85</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E18">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E19">
         <v>1.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E20">
         <v>3.75</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E21">
         <v>5.85</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E22">
         <v>10.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E23">
         <v>7.8</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E24">
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E25">
         <v>3.75</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E26">
         <v>5.85</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E27">
         <v>10.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E28">
         <v>7.8</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C29">
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E29">
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C30">
         <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E30">
         <v>3.75</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E31">
         <v>5.85</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C32">
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E32">
         <v>7.8</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C33">
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E33">
         <v>7.6</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C34">
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E34">
         <v>1.2</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C35">
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E35">
         <v>0.6</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C36">
         <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E36">
         <v>3.75</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C37">
         <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E37">
         <v>5.85</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C38">
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E38">
         <v>7.8</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C39">
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E39">
         <v>7.6</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E40">
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C41">
         <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E41">
         <v>0.6</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C42">
         <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E42">
         <v>3.75</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C43">
         <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E43">
         <v>5.85</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C44">
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E44">
         <v>8.35</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C45">
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E45">
         <v>7.6</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C46">
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E46">
         <v>0.85</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C47">
         <v>90</v>
       </c>
       <c r="D47" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E47">
         <v>3.75</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C48">
         <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E48">
         <v>5.85</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C49">
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E49">
         <v>8.35</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C50">
         <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E50">
         <v>7.6</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C51">
         <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E51">
         <v>0.85</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>45</v>
       </c>
       <c r="D52" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E52">
         <v>3.75</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C53">
         <v>90</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E53">
         <v>5.85</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C54">
         <v>60</v>
       </c>
       <c r="D54" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E54">
         <v>5.5</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C55">
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E55">
         <v>7.6</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C56">
         <v>43</v>
       </c>
       <c r="D56" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E56">
         <v>0.6</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C57">
         <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E57">
         <v>3.75</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E58">
         <v>5.85</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C59">
         <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E59">
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C60">
         <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E60">
         <v>7.6</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C61">
         <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E61">
         <v>0.6</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E62">
         <v>3.75</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C63">
         <v>90</v>
       </c>
       <c r="D63" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E63">
         <v>5.85</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C64">
         <v>14</v>
       </c>
       <c r="D64" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E64">
-        <v>16.4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C65">
         <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E65">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C66">
         <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E66">
         <v>15.25</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C67">
         <v>90</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E67">
         <v>3.75</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C68">
         <v>120</v>
       </c>
       <c r="D68" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E68">
         <v>5.85</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C69">
         <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E69">
-        <v>16.4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C70">
         <v>90</v>
       </c>
       <c r="D70" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E70">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C71">
         <v>35</v>
       </c>
       <c r="D71" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E71">
         <v>15.25</v>
       </c>
     </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <v>22.5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>51</v>
+      </c>
+      <c r="E73">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74">
+        <v>35</v>
+      </c>
+      <c r="D74" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75">
+        <v>30</v>
+      </c>
+      <c r="D75" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>40</v>
+      </c>
+      <c r="C77">
+        <v>40</v>
+      </c>
+      <c r="D77" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" t="s">
+        <v>41</v>
+      </c>
+      <c r="C78">
+        <v>55</v>
+      </c>
+      <c r="D78" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80">
+        <v>20</v>
+      </c>
+      <c r="D80" t="s">
+        <v>51</v>
+      </c>
+      <c r="E80">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C81">
+        <v>20</v>
+      </c>
+      <c r="D81" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>43</v>
+      </c>
+      <c r="C82">
+        <v>15</v>
+      </c>
+      <c r="D82" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C83">
+        <v>15</v>
+      </c>
+      <c r="D83" t="s">
+        <v>51</v>
+      </c>
+      <c r="E83">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" t="s">
+        <v>45</v>
+      </c>
+      <c r="C84">
+        <v>20</v>
+      </c>
+      <c r="D84" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C85">
+        <v>25</v>
+      </c>
+      <c r="D85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E85">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86">
+        <v>20</v>
+      </c>
+      <c r="D86" t="s">
+        <v>51</v>
+      </c>
+      <c r="E86">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87">
+        <v>20</v>
+      </c>
+      <c r="D87" t="s">
+        <v>51</v>
+      </c>
+      <c r="E87">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88">
+        <v>25</v>
+      </c>
+      <c r="D88" t="s">
+        <v>51</v>
+      </c>
+      <c r="E88">
+        <v>28.33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89">
+        <v>20</v>
+      </c>
+      <c r="D89" t="s">
+        <v>51</v>
+      </c>
+      <c r="E89">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" t="s">
+        <v>47</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90" t="s">
+        <v>51</v>
+      </c>
+      <c r="E90">
+        <v>6.71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91">
+        <v>30</v>
+      </c>
+      <c r="D91" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92">
+        <v>25</v>
+      </c>
+      <c r="D92" t="s">
+        <v>51</v>
+      </c>
+      <c r="E92">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93">
+        <v>40</v>
+      </c>
+      <c r="D93" t="s">
+        <v>51</v>
+      </c>
+      <c r="E93">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B94" t="s">
+        <v>50</v>
+      </c>
+      <c r="C94">
+        <v>45</v>
+      </c>
+      <c r="D94" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>19</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95">
+        <v>30</v>
+      </c>
+      <c r="D95" t="s">
+        <v>51</v>
+      </c>
+      <c r="E95">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>19</v>
+      </c>
+      <c r="B96" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96">
+        <v>20</v>
+      </c>
+      <c r="D96" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97">
+        <v>35</v>
+      </c>
+      <c r="D97" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98">
+        <v>40</v>
+      </c>
+      <c r="D98" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" t="s">
+        <v>35</v>
+      </c>
+      <c r="C99">
+        <v>35</v>
+      </c>
+      <c r="D99" t="s">
+        <v>51</v>
+      </c>
+      <c r="E99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" t="s">
+        <v>38</v>
+      </c>
+      <c r="C100">
+        <v>30</v>
+      </c>
+      <c r="D100" t="s">
+        <v>51</v>
+      </c>
+      <c r="E100">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>39</v>
+      </c>
+      <c r="C101">
+        <v>40</v>
+      </c>
+      <c r="D101" t="s">
+        <v>51</v>
+      </c>
+      <c r="E101">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>40</v>
+      </c>
+      <c r="C102">
+        <v>40</v>
+      </c>
+      <c r="D102" t="s">
+        <v>51</v>
+      </c>
+      <c r="E102">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103">
+        <v>55</v>
+      </c>
+      <c r="D103" t="s">
+        <v>51</v>
+      </c>
+      <c r="E103">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104">
+        <v>40</v>
+      </c>
+      <c r="D104" t="s">
+        <v>51</v>
+      </c>
+      <c r="E104">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" t="s">
+        <v>24</v>
+      </c>
+      <c r="C105">
+        <v>20</v>
+      </c>
+      <c r="D105" t="s">
+        <v>51</v>
+      </c>
+      <c r="E105">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" t="s">
+        <v>42</v>
+      </c>
+      <c r="C106">
+        <v>20</v>
+      </c>
+      <c r="D106" t="s">
+        <v>51</v>
+      </c>
+      <c r="E106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>43</v>
+      </c>
+      <c r="C107">
+        <v>15</v>
+      </c>
+      <c r="D107" t="s">
+        <v>51</v>
+      </c>
+      <c r="E107">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" t="s">
+        <v>44</v>
+      </c>
+      <c r="C108">
+        <v>15</v>
+      </c>
+      <c r="D108" t="s">
+        <v>51</v>
+      </c>
+      <c r="E108">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>20</v>
+      </c>
+      <c r="B109" t="s">
+        <v>45</v>
+      </c>
+      <c r="C109">
+        <v>20</v>
+      </c>
+      <c r="D109" t="s">
+        <v>51</v>
+      </c>
+      <c r="E109">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" t="s">
+        <v>46</v>
+      </c>
+      <c r="C110">
+        <v>25</v>
+      </c>
+      <c r="D110" t="s">
+        <v>51</v>
+      </c>
+      <c r="E110">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111" t="s">
+        <v>30</v>
+      </c>
+      <c r="C111">
+        <v>20</v>
+      </c>
+      <c r="D111" t="s">
+        <v>51</v>
+      </c>
+      <c r="E111">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>20</v>
+      </c>
+      <c r="B112" t="s">
+        <v>31</v>
+      </c>
+      <c r="C112">
+        <v>20</v>
+      </c>
+      <c r="D112" t="s">
+        <v>51</v>
+      </c>
+      <c r="E112">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>20</v>
+      </c>
+      <c r="B113" t="s">
+        <v>32</v>
+      </c>
+      <c r="C113">
+        <v>25</v>
+      </c>
+      <c r="D113" t="s">
+        <v>51</v>
+      </c>
+      <c r="E113">
+        <v>28.33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114" t="s">
+        <v>26</v>
+      </c>
+      <c r="C114">
+        <v>20</v>
+      </c>
+      <c r="D114" t="s">
+        <v>51</v>
+      </c>
+      <c r="E114">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>20</v>
+      </c>
+      <c r="B115" t="s">
+        <v>47</v>
+      </c>
+      <c r="C115">
+        <v>4</v>
+      </c>
+      <c r="D115" t="s">
+        <v>51</v>
+      </c>
+      <c r="E115">
+        <v>6.71</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116">
+        <v>30</v>
+      </c>
+      <c r="D116" t="s">
+        <v>51</v>
+      </c>
+      <c r="E116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117" t="s">
+        <v>49</v>
+      </c>
+      <c r="C117">
+        <v>25</v>
+      </c>
+      <c r="D117" t="s">
+        <v>51</v>
+      </c>
+      <c r="E117">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>20</v>
+      </c>
+      <c r="B118" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118">
+        <v>40</v>
+      </c>
+      <c r="D118" t="s">
+        <v>51</v>
+      </c>
+      <c r="E118">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>20</v>
+      </c>
+      <c r="B119" t="s">
+        <v>50</v>
+      </c>
+      <c r="C119">
+        <v>45</v>
+      </c>
+      <c r="D119" t="s">
+        <v>51</v>
+      </c>
+      <c r="E119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>20</v>
+      </c>
+      <c r="B120" t="s">
+        <v>23</v>
+      </c>
+      <c r="C120">
+        <v>30</v>
+      </c>
+      <c r="D120" t="s">
+        <v>51</v>
+      </c>
+      <c r="E120">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>20</v>
+      </c>
+      <c r="B121" t="s">
+        <v>36</v>
+      </c>
+      <c r="C121">
+        <v>20</v>
+      </c>
+      <c r="D121" t="s">
+        <v>51</v>
+      </c>
+      <c r="E121">
+        <v>15.25</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:A121" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>